<commit_message>
Improve image download with SSL handling and path tracking
</commit_message>
<xml_diff>
--- a/DSSP.xlsx
+++ b/DSSP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Find_IMG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896DC580-6C29-43F7-A814-DBE46010C1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810F4E16-F8F4-4CA9-A26F-082ECDC24B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>barcode</t>
   </si>
@@ -34,28 +34,7 @@
     <t>SRM Neutrogena Ngừa Mụn 100ml</t>
   </si>
   <si>
-    <t>Sáp KM nam Old Spice Bearglove 73g</t>
-  </si>
-  <si>
-    <t>Nước cốt dừa Aroy 165ml</t>
-  </si>
-  <si>
-    <t>DG Ogx phục hồi hư tổn 385ml</t>
-  </si>
-  <si>
-    <t>DG OGX Biotin &amp; Collagen 385ml</t>
-  </si>
-  <si>
-    <t>ST Olay ngừa lão hoá vitaminE 650ml</t>
-  </si>
-  <si>
-    <t>BCR Chanh 175G</t>
-  </si>
-  <si>
-    <t>BCR Bạc Hà 175G</t>
-  </si>
-  <si>
-    <t>Cước cọ rửa mút HHD gói 3 miếng</t>
+    <t>hinh_anh_san_pham\SRM_Neutrogena_Ngua_Mun_100ml.jpg</t>
   </si>
 </sst>
 </file>
@@ -444,16 +423,16 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="64.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.88671875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -474,78 +453,44 @@
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2"/>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2">
-        <v>12044039632</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2">
-        <v>16229001704</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2">
-        <v>22796916112</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:3" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="2">
-        <v>22796916709</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6"/>
-    </row>
-    <row r="7" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="2">
-        <v>37000974734</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="2">
-        <v>47400245105</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="2">
-        <v>47400247307</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="2">
-        <v>51131596733</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(find.py): Download 3 images per product with sequential numbering
- Add support for downloading 3 images per product instead of 1
- Implement sequential numbering for downloaded images (_1, _2, _3)
- Update download_image() function to accept image_number parameter
- Modify image filename generation to include sequential number suffix
- Refactor write_image_path_to_excel() to write_image_paths_to_excel() for multiple columns
- Update Excel integration to write image paths to columns C, D, E (img1, img2, img3)
- Enhance image search logic to find and click 3 clickable images instead of 1
- Update README.md with new feature documentation and usage examples
- Update DSSP.xlsx with sample data reflecting new 3-image structure
- Add v2.0.0 changelog entry documenting the multi-image download feature
</commit_message>
<xml_diff>
--- a/DSSP.xlsx
+++ b/DSSP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Find_IMG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rocket global\POS\Find_IMG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810F4E16-F8F4-4CA9-A26F-082ECDC24B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878DC5A0-67BA-4046-9CE2-B86216A8C016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5895" yWindow="2970" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>barcode</t>
   </si>
@@ -28,13 +28,61 @@
     <t>name</t>
   </si>
   <si>
-    <t>img</t>
-  </si>
-  <si>
-    <t>SRM Neutrogena Ngừa Mụn 100ml</t>
-  </si>
-  <si>
-    <t>hinh_anh_san_pham\SRM_Neutrogena_Ngua_Mun_100ml.jpg</t>
+    <t>KDR Colgate TOT ActiveFresh 150g</t>
+  </si>
+  <si>
+    <t>hinh_anh_san_pham\KDR_Colgate_TOT_ActiveFresh_150g_1.jpg</t>
+  </si>
+  <si>
+    <t>hinh_anh_san_pham\KDR_Colgate_TOT_ActiveFresh_150g_2.jpg</t>
+  </si>
+  <si>
+    <t>hinh_anh_san_pham\KDR_Colgate_TOT_ActiveFresh_150g_3.jpg</t>
+  </si>
+  <si>
+    <t>KDR Colgate CSPR Comp Protect 110g</t>
+  </si>
+  <si>
+    <t>hinh_anh_san_pham\KDR_Colgate_CSPR_Comp_Protect_110g_1.jpg</t>
+  </si>
+  <si>
+    <t>hinh_anh_san_pham\KDR_Colgate_CSPR_Comp_Protect_110g_2.jpg</t>
+  </si>
+  <si>
+    <t>hinh_anh_san_pham\KDR_Colgate_CSPR_Comp_Protect_110g_3.jpg</t>
+  </si>
+  <si>
+    <t>BCDR Colgate SlimSoft Charcoal 1PK</t>
+  </si>
+  <si>
+    <t>hinh_anh_san_pham\BCDR_Colgate_SlimSoft_Charcoal_1PK_1.jpg</t>
+  </si>
+  <si>
+    <t>hinh_anh_san_pham\BCDR_Colgate_SlimSoft_Charcoal_1PK_2.jpg</t>
+  </si>
+  <si>
+    <t>hinh_anh_san_pham\BCDR_Colgate_SlimSoft_Charcoal_1PK_3.jpg</t>
+  </si>
+  <si>
+    <t>BCDR Colgate 360 Char Spiral 2</t>
+  </si>
+  <si>
+    <t>hinh_anh_san_pham\BCDR_Colgate_360_Char_Spiral_2_1.jpg</t>
+  </si>
+  <si>
+    <t>hinh_anh_san_pham\BCDR_Colgate_360_Char_Spiral_2_2.jpg</t>
+  </si>
+  <si>
+    <t>hinh_anh_san_pham\BCDR_Colgate_360_Char_Spiral_2_3.jpg</t>
+  </si>
+  <si>
+    <t>img1</t>
+  </si>
+  <si>
+    <t>img2</t>
+  </si>
+  <si>
+    <t>img3</t>
   </si>
 </sst>
 </file>
@@ -420,22 +468,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="64.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.88671875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="64.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="62.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,49 +492,100 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="67.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>8850006325636</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2">
-        <v>70501017104</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="67.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>8850006327647</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="41.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>8850006331866</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>8850006332030</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:3" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:3" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:3" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:3" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
     </row>

</xml_diff>

<commit_message>
feat(find.py): Add multiprocessing support with 3 parallel browsers
- Implement ThreadPoolExecutor for concurrent product processing
- Add NUM_WORKERS configuration (default 3, adjustable for RAM availability)
- Create worker-specific Selenium profiles to prevent conflicts
- Add threading.Lock for thread-safe Excel writing operations
- Reduce delay from 3-5s to 2-3s per product due to parallel execution
- Position browser windows differently for each worker for easier monitoring
- Update .gitignore to track selenium_profile_worker_* directories
- Add multiprocessing documentation to README with RAM recommendations
- Update DSSP.xlsx with new product data
- Add v2.1.0 changelog entry documenting performance improvements
- Achieves ~3x speed improvement by running 3 Chrome instances simultaneously
</commit_message>
<xml_diff>
--- a/DSSP.xlsx
+++ b/DSSP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rocket global\POS\Find_IMG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878DC5A0-67BA-4046-9CE2-B86216A8C016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FA8C70-1991-4F7F-AACF-079584201A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5895" yWindow="2970" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>barcode</t>
   </si>
@@ -28,54 +28,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>KDR Colgate TOT ActiveFresh 150g</t>
-  </si>
-  <si>
-    <t>hinh_anh_san_pham\KDR_Colgate_TOT_ActiveFresh_150g_1.jpg</t>
-  </si>
-  <si>
-    <t>hinh_anh_san_pham\KDR_Colgate_TOT_ActiveFresh_150g_2.jpg</t>
-  </si>
-  <si>
-    <t>hinh_anh_san_pham\KDR_Colgate_TOT_ActiveFresh_150g_3.jpg</t>
-  </si>
-  <si>
-    <t>KDR Colgate CSPR Comp Protect 110g</t>
-  </si>
-  <si>
-    <t>hinh_anh_san_pham\KDR_Colgate_CSPR_Comp_Protect_110g_1.jpg</t>
-  </si>
-  <si>
-    <t>hinh_anh_san_pham\KDR_Colgate_CSPR_Comp_Protect_110g_2.jpg</t>
-  </si>
-  <si>
-    <t>hinh_anh_san_pham\KDR_Colgate_CSPR_Comp_Protect_110g_3.jpg</t>
-  </si>
-  <si>
-    <t>BCDR Colgate SlimSoft Charcoal 1PK</t>
-  </si>
-  <si>
-    <t>hinh_anh_san_pham\BCDR_Colgate_SlimSoft_Charcoal_1PK_1.jpg</t>
-  </si>
-  <si>
-    <t>hinh_anh_san_pham\BCDR_Colgate_SlimSoft_Charcoal_1PK_2.jpg</t>
-  </si>
-  <si>
-    <t>hinh_anh_san_pham\BCDR_Colgate_SlimSoft_Charcoal_1PK_3.jpg</t>
-  </si>
-  <si>
-    <t>BCDR Colgate 360 Char Spiral 2</t>
-  </si>
-  <si>
-    <t>hinh_anh_san_pham\BCDR_Colgate_360_Char_Spiral_2_1.jpg</t>
-  </si>
-  <si>
-    <t>hinh_anh_san_pham\BCDR_Colgate_360_Char_Spiral_2_2.jpg</t>
-  </si>
-  <si>
-    <t>hinh_anh_san_pham\BCDR_Colgate_360_Char_Spiral_2_3.jpg</t>
-  </si>
-  <si>
     <t>img1</t>
   </si>
   <si>
@@ -83,6 +35,213 @@
   </si>
   <si>
     <t>img3</t>
+  </si>
+  <si>
+    <t>ST Chua Sữa &amp; Gạo 500ml</t>
+  </si>
+  <si>
+    <t>NHH Neutrogena không cồn 150ml</t>
+  </si>
+  <si>
+    <t>SRM XMen Men Deep Cleanse 100G</t>
+  </si>
+  <si>
+    <t>NTT Neutrogena Micellar 400ml</t>
+  </si>
+  <si>
+    <t>SRM Neutrogena Kiểm Soát Nhờn 100ml</t>
+  </si>
+  <si>
+    <t>NSM Listerine Coolmint 750ml</t>
+  </si>
+  <si>
+    <t>NSM Listerine Green Tea 750ml</t>
+  </si>
+  <si>
+    <t>NSM Listerine Green Tea 250ml</t>
+  </si>
+  <si>
+    <t>NSM Listerine Total Care Zero 750ml</t>
+  </si>
+  <si>
+    <t>Listerine Total Care Zero 250ml</t>
+  </si>
+  <si>
+    <t>Listerine Coolmint 250ml</t>
+  </si>
+  <si>
+    <t>Listerine Kid 250ml</t>
+  </si>
+  <si>
+    <t>SRM NIVEA Đất Sét 100g</t>
+  </si>
+  <si>
+    <t>NTT NIVEA Dưỡng Ẩm 200ml</t>
+  </si>
+  <si>
+    <t>NTT NIVEA Kiểm Soát Nhờn 200ml</t>
+  </si>
+  <si>
+    <t>NTT NIVEA Kiểm Soát Nhờn 125ml</t>
+  </si>
+  <si>
+    <t>NTT Ngừa Mụn 125ml</t>
+  </si>
+  <si>
+    <t>NTT Ngừa Mụn 200ml</t>
+  </si>
+  <si>
+    <t>KDA NIVEA Dưỡng Ẩm 60ml</t>
+  </si>
+  <si>
+    <t>SDT NIVEA Phục Hồi 350ml</t>
+  </si>
+  <si>
+    <t>NTT NIVEA Ngừa Mụn 400ml</t>
+  </si>
+  <si>
+    <t>NTT NIVEA Dưỡng Ẩm 400ml</t>
+  </si>
+  <si>
+    <t>SRM NIVEA Himalaya 100g</t>
+  </si>
+  <si>
+    <t>SRM Derma Acne Care 90ml</t>
+  </si>
+  <si>
+    <t>NTT Derma Acne Care 400ml</t>
+  </si>
+  <si>
+    <t>XNM NIVEA Nữ Mịn Mượt 150ml</t>
+  </si>
+  <si>
+    <t>LNM Ngọc Trai Mịn Mượt 50ml</t>
+  </si>
+  <si>
+    <t>SRM Sáng Da Bọt Mịn 100ml</t>
+  </si>
+  <si>
+    <t>SRM Sáng Da Bọt Khí 100ml</t>
+  </si>
+  <si>
+    <t>LNM NIVEA Nữ Giảm Ố Vàng 25ml</t>
+  </si>
+  <si>
+    <t>XNM NIVEA Ngọc Trai 150ml</t>
+  </si>
+  <si>
+    <t>Son NIVEA Dưỡng Ẩm 5.5ml</t>
+  </si>
+  <si>
+    <t>Son NIVEA Dưỡng Ẩm 4.8g</t>
+  </si>
+  <si>
+    <t>Bột cacao Ovaltine 1kg</t>
+  </si>
+  <si>
+    <t>KDR Sensodyne Mát Lạnh 160g</t>
+  </si>
+  <si>
+    <t>KDR Sensodyne Bảo Vệ Nướu 100g</t>
+  </si>
+  <si>
+    <t>KDR Sensodyne Trắng Sáng 160g</t>
+  </si>
+  <si>
+    <t>Bún Gạo Khô Waiwai 200g</t>
+  </si>
+  <si>
+    <t>Miến Đậu Xanh Song Long 200g</t>
+  </si>
+  <si>
+    <t>Glade _ Sáp thơm biển phiêu bồng 180g</t>
+  </si>
+  <si>
+    <t>Glade Sáp Anh Đào 180g</t>
+  </si>
+  <si>
+    <t>Glade Sáp thơm anh đào 180g</t>
+  </si>
+  <si>
+    <t>Glade Sáp TrầmHương 180g</t>
+  </si>
+  <si>
+    <t>NTL Redbull Thái Kẽm 250ml</t>
+  </si>
+  <si>
+    <t>Kẹo nhân cà phê Amira 300g</t>
+  </si>
+  <si>
+    <t>Kẹo mận Amira 250g</t>
+  </si>
+  <si>
+    <t>Bánh xốp Imperial socola quýt 100g</t>
+  </si>
+  <si>
+    <t>Miến Đậu Xanh Pine Brand 80gr</t>
+  </si>
+  <si>
+    <t>Kẹo chanh muối vitamin C 120g</t>
+  </si>
+  <si>
+    <t>BB Stax Tự Nhiên 100g</t>
+  </si>
+  <si>
+    <t>BB Stax Tôm 100g</t>
+  </si>
+  <si>
+    <t>BB Stax Kem 100g</t>
+  </si>
+  <si>
+    <t>BB Stax Mực 100g</t>
+  </si>
+  <si>
+    <t>BB Stax Tôm 42g</t>
+  </si>
+  <si>
+    <t>BB Stax Kem 42g</t>
+  </si>
+  <si>
+    <t>BB Stax Tự Nhiên 42g</t>
+  </si>
+  <si>
+    <t>KU Pureen 80T (Trộn)</t>
+  </si>
+  <si>
+    <t>Kẹo ngậm D.Mint chanh 23g</t>
+  </si>
+  <si>
+    <t>Mì gói Tomyum Mama 55G</t>
+  </si>
+  <si>
+    <t>BCDR Sensodyne Repair &amp; Protect ExSoft</t>
+  </si>
+  <si>
+    <t>KDR Sensodyne Bảo Vệ Nướu 160g</t>
+  </si>
+  <si>
+    <t>KDR Sensodyne reparir &amp; protect soft</t>
+  </si>
+  <si>
+    <t>BCDR Sensodyne Repair &amp; Protect Extra Soft</t>
+  </si>
+  <si>
+    <t>KDR Sensodyne Repair &amp; Protect 100g</t>
+  </si>
+  <si>
+    <t>KDR Sensodyne Rapid Action 100g</t>
+  </si>
+  <si>
+    <t>Bánh Pocky Kem Choco 40g</t>
+  </si>
+  <si>
+    <t>Bánh Pocky Kem Dâu 38g</t>
+  </si>
+  <si>
+    <t>Bánh Pocky Kem Trà Xanh Vị Sữa 35g</t>
+  </si>
+  <si>
+    <t>Bánh Pocky Kem Cookies &amp; Cream 40g</t>
   </si>
 </sst>
 </file>
@@ -468,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -480,8 +639,8 @@
     <col min="2" max="2" width="28.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="64.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="62.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="9" width="8.85546875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -492,105 +651,664 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="67.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>8850006325636</v>
+        <v>8850007090281</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
         <v>5</v>
       </c>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
     </row>
     <row r="3" spans="1:5" ht="67.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>8850006327647</v>
+        <v>8850007540212</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
     </row>
     <row r="4" spans="1:5" ht="41.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>8850006331866</v>
+        <v>8850007541684</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
     </row>
     <row r="5" spans="1:5" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>8850006332030</v>
+        <v>8850007542827</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+    </row>
+    <row r="6" spans="1:5" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>8850007543138</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+    </row>
+    <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>8850007800071</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+    </row>
+    <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>8850007812524</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+    </row>
+    <row r="9" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8850007812562</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+    </row>
+    <row r="10" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>8850007812760</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+    </row>
+    <row r="11" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>8850007812876</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+    </row>
+    <row r="12" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>8850007813040</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+    </row>
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>8850007814696</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+    </row>
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>8850029000114</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+    </row>
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>8850029010656</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+    </row>
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>8850029015194</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+    </row>
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>8850029015200</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+    </row>
+    <row r="18" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>8850029017730</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+    </row>
+    <row r="19" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>8850029017747</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+    </row>
+    <row r="20" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>8850029018065</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+    </row>
+    <row r="21" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>8850029023076</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+    </row>
+    <row r="22" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>8850029026923</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+    </row>
+    <row r="23" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>8850029026947</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+    </row>
+    <row r="24" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>8850029032856</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+    </row>
+    <row r="25" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>8850029036410</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>8850029036434</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>8850029037660</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>8850029037684</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>8850029043647</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+    </row>
+    <row r="30" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
+        <v>8850029043654</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+    </row>
+    <row r="31" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>8850029212333</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>8850029212746</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>8850029850009</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>8850029850726</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>8850086194016</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>8850090113164</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>8850090114109</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>8850090400424</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>8850100206022</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>8850122101046</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>8850175010500</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>8850175020479</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="2">
+        <v>8850175020868</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="2">
+        <v>8850175024002</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>8850228007617</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="2">
+        <v>8850305310487</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="2">
+        <v>8850305310852</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>8850332223248</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="2">
+        <v>8850372000403</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="2">
+        <v>8850632205159</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="2">
+        <v>8850718803347</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="2">
+        <v>8850718803873</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="2">
+        <v>8850718804573</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="2">
+        <v>8850718808410</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="2">
+        <v>8850718816057</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="2">
+        <v>8850718816064</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="2">
+        <v>8850718816071</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="2">
+        <v>8850848011162</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="2">
+        <v>8850939920533</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="2">
+        <v>8850987101021</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="2">
+        <v>8851007108112</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="2">
+        <v>8851007110498</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="2">
+        <v>8851007142413</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="2">
+        <v>8851007158995</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="2">
+        <v>8851007198038</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="2">
+        <v>8851007198397</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="2">
+        <v>8851007199332</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="2">
+        <v>8851019310190</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="2">
+        <v>8851019310206</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="2">
+        <v>8851019500164</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="2">
+        <v>8851019500195</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>